<commit_message>
TODO: notification font, clean code
</commit_message>
<xml_diff>
--- a/2.Development Schedule and Milestones.xlsx
+++ b/2.Development Schedule and Milestones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COMP8047_Major_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC3A8AE-7B8F-4462-87BB-36AADFBAAE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93003DD4-8B8B-4041-9AB9-13F983BDE4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9435" yWindow="3000" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -286,7 +286,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,8 +299,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8A2A2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -308,30 +326,337 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="2" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="2" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE8A2A2"/>
+      <color rgb="FFCD3333"/>
+      <color rgb="FFFF6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1074,6 +1399,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1081,7 +1407,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1967,984 +2292,985 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E8"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.375" style="2" customWidth="1"/>
     <col min="3" max="3" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1" s="22">
         <f>SUM(B2,B9,B15,B27,B33,B39,B45,B48)</f>
         <v>545</v>
       </c>
-      <c r="D1" s="8">
+      <c r="C1" s="23"/>
+      <c r="D1" s="24">
         <f>D2</f>
         <v>45831</v>
       </c>
-      <c r="E1" s="8">
+      <c r="E1" s="25">
         <f>E48</f>
         <v>45940</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="37">
         <f>SUM(B3:B8)</f>
         <v>55</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="38">
         <f>SUM(C3:C8)</f>
         <v>11</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="39">
         <f>D3</f>
         <v>45831</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="40">
         <f>E8</f>
         <v>45842</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="7">
         <v>5</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="6">
         <v>1</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="8">
         <v>45831</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="13">
         <f>D3+C3</f>
         <v>45832</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="7">
         <v>10</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="6">
         <v>2</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="8">
         <f>E3</f>
         <v>45832</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="13">
         <f t="shared" ref="E4:E8" si="0">D4+C4</f>
         <v>45834</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="7">
         <v>10</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="6">
         <v>2</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="8">
         <f t="shared" ref="D5:D8" si="1">E4</f>
         <v>45834</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="13">
         <f t="shared" si="0"/>
         <v>45836</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="7">
         <v>5</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="6">
         <v>1</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="8">
         <f t="shared" si="1"/>
         <v>45836</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="13">
         <f t="shared" si="0"/>
         <v>45837</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="7">
         <v>15</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="6">
         <v>3</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="8">
         <f t="shared" si="1"/>
         <v>45837</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="13">
         <f t="shared" si="0"/>
         <v>45840</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="27">
         <v>10</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="28">
         <v>2</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="29">
         <f t="shared" si="1"/>
         <v>45840</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="30">
         <f t="shared" si="0"/>
         <v>45842</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="42">
         <f>SUM(B10:B14)</f>
         <v>55</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="43">
         <f>SUM(C10:C14)</f>
         <v>11</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="44">
         <f>D10</f>
         <v>45842</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="45">
         <f>E14</f>
         <v>45853</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="10">
         <v>10</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="9">
         <v>2</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="11">
         <f>E8</f>
         <v>45842</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="15">
         <f>D10+C10</f>
         <v>45844</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="10">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="9">
         <v>2</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="11">
         <f>E10</f>
         <v>45844</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="15">
         <f t="shared" ref="E11:E14" si="2">D11+C11</f>
         <v>45846</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="10">
         <v>15</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="9">
         <v>3</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="11">
         <f t="shared" ref="D12:D14" si="3">E11</f>
         <v>45846</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="15">
         <f t="shared" si="2"/>
         <v>45849</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="10">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="9">
         <v>2</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="11">
         <f t="shared" si="3"/>
         <v>45849</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="15">
         <f t="shared" si="2"/>
         <v>45851</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="32">
         <v>10</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="33">
         <v>2</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="34">
         <f t="shared" si="3"/>
         <v>45851</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="35">
         <f t="shared" si="2"/>
         <v>45853</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="37">
         <f>SUM(B16:B26)</f>
         <v>115</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="38">
         <f>SUM(C16:C26)</f>
         <v>23</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="39">
         <f>D16</f>
         <v>45853</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="40">
         <f>E26</f>
         <v>45876</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="10">
         <v>10</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="9">
         <v>2</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="11">
         <f>E14</f>
         <v>45853</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="15">
         <f>D16+C16</f>
         <v>45855</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="10">
         <v>10</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="9">
         <v>2</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="11">
         <f>E16</f>
         <v>45855</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="15">
         <f t="shared" ref="E17:E26" si="4">D17+C17</f>
         <v>45857</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="10">
         <v>15</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="9">
         <v>3</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="11">
         <f t="shared" ref="D18:D26" si="5">E17</f>
         <v>45857</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="15">
         <f t="shared" si="4"/>
         <v>45860</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="10">
         <v>10</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="9">
         <v>2</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="11">
         <f t="shared" si="5"/>
         <v>45860</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="15">
         <f t="shared" si="4"/>
         <v>45862</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="10">
         <v>10</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="9">
         <v>2</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="11">
         <f t="shared" si="5"/>
         <v>45862</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="15">
         <f t="shared" si="4"/>
         <v>45864</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="10">
         <v>10</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="9">
         <v>2</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="11">
         <f t="shared" si="5"/>
         <v>45864</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="15">
         <f t="shared" si="4"/>
         <v>45866</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="10">
         <v>10</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="9">
         <v>2</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="11">
         <f t="shared" si="5"/>
         <v>45866</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="15">
         <f t="shared" si="4"/>
         <v>45868</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="10">
         <v>10</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="9">
         <v>2</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="11">
         <f t="shared" si="5"/>
         <v>45868</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="15">
         <f t="shared" si="4"/>
         <v>45870</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="7">
         <v>10</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="6">
         <v>2</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="8">
         <f t="shared" si="5"/>
         <v>45870</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="13">
         <f t="shared" si="4"/>
         <v>45872</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="7">
         <v>10</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="6">
         <v>2</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="8">
         <f t="shared" si="5"/>
         <v>45872</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="13">
         <f t="shared" si="4"/>
         <v>45874</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="27">
         <v>10</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="28">
         <v>2</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="29">
         <f t="shared" si="5"/>
         <v>45874</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="30">
         <f t="shared" si="4"/>
         <v>45876</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="42">
         <f>SUM(B28:B32)</f>
         <v>40</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="43">
         <f>SUM(C28:C32)</f>
         <v>8</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="44">
         <f>D28</f>
         <v>45876</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="45">
         <f>E32</f>
         <v>45884</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="10">
         <v>5</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="9">
         <v>1</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="11">
         <f>E26</f>
         <v>45876</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="15">
         <f>D28+C28</f>
         <v>45877</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="10">
         <v>5</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="9">
         <v>1</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="11">
         <f>E28</f>
         <v>45877</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="15">
         <f t="shared" ref="E29:E32" si="6">D29+C29</f>
         <v>45878</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="10">
         <v>10</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="9">
         <v>2</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="11">
         <f t="shared" ref="D30:D32" si="7">E29</f>
         <v>45878</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="15">
         <f t="shared" si="6"/>
         <v>45880</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="10">
         <v>10</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="9">
         <v>2</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="11">
         <f t="shared" si="7"/>
         <v>45880</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="15">
         <f t="shared" si="6"/>
         <v>45882</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="32">
         <v>10</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="33">
         <v>2</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="34">
         <f t="shared" si="7"/>
         <v>45882</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="35">
         <f t="shared" si="6"/>
         <v>45884</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="37">
         <f>SUM(B34:B38)</f>
         <v>40</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="38">
         <f>SUM(C34:C38)</f>
         <v>8</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="39">
         <f>D34</f>
         <v>45884</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="40">
         <f>E38</f>
         <v>45892</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="A34" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="10">
         <v>5</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="9">
         <v>1</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="11">
         <f>E32</f>
         <v>45884</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="15">
         <f>D34+C34</f>
         <v>45885</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="A35" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="10">
         <v>5</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="9">
         <v>1</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="11">
         <f>E34</f>
         <v>45885</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="15">
         <f t="shared" ref="E35:E38" si="8">D35+C35</f>
         <v>45886</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="A36" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="10">
         <v>10</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="9">
         <v>2</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="11">
         <f t="shared" ref="D36:D38" si="9">E35</f>
         <v>45886</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="15">
         <f t="shared" si="8"/>
         <v>45888</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="A37" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="10">
         <v>10</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="9">
         <v>2</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="11">
         <f t="shared" si="9"/>
         <v>45888</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="15">
         <f t="shared" si="8"/>
         <v>45890</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="57">
         <v>10</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="58">
         <v>2</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="59">
         <f t="shared" si="9"/>
         <v>45890</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="60">
         <f t="shared" si="8"/>
         <v>45892</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="42">
         <f>SUM(B40:B44)</f>
         <v>40</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="43">
         <f>SUM(C40:C44)</f>
         <v>8</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="44">
         <f>D40</f>
         <v>45892</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="45">
         <f>E44</f>
         <v>45900</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="A40" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="10">
         <v>5</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="9">
         <v>1</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="11">
         <f>E38</f>
         <v>45892</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="15">
         <f>D40+C40</f>
         <v>45893</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="A41" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="10">
         <v>5</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="9">
         <v>1</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="11">
         <f>E40</f>
         <v>45893</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="15">
         <f t="shared" ref="E41:E44" si="10">D41+C41</f>
         <v>45894</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="10">
         <v>10</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="9">
         <v>2</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="11">
         <f>E41</f>
         <v>45894</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="15">
         <f t="shared" si="10"/>
         <v>45896</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="10">
         <v>10</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="9">
         <v>2</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="11">
         <f t="shared" ref="D43:D44" si="11">E42</f>
         <v>45896</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="15">
         <f t="shared" si="10"/>
         <v>45898</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="32">
         <v>10</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="33">
         <v>2</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="34">
         <f t="shared" si="11"/>
         <v>45898</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="35">
         <f t="shared" si="10"/>
         <v>45900</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="37">
         <f>SUM(B46:B47)</f>
         <v>35</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="38">
         <f>SUM(C46:C47)</f>
         <v>7</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="39">
         <f>D46</f>
         <v>45900</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="40">
         <f>E47</f>
         <v>45907</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="A46" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="47">
         <v>15</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="48">
         <v>3</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="49">
         <f>E44</f>
         <v>45900</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="50">
         <f>D46+C46</f>
         <v>45903</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="52">
         <v>20</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="53">
         <v>4</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="54">
         <f>E46</f>
         <v>45903</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="55">
         <f t="shared" ref="E47" si="12">D47+C47</f>
         <v>45907</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="42">
         <f>SUM(B49:B50)</f>
         <v>165</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="43">
         <f>SUM(C49:C50)</f>
         <v>33</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="44">
         <f>D49</f>
         <v>45907</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48" s="45">
         <f>E50</f>
         <v>45940</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="A49" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="47">
         <v>15</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="48">
         <v>3</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="49">
         <f>E47</f>
         <v>45907</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="50">
         <f t="shared" ref="E49:E50" si="13">D49+C49</f>
         <v>45910</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="17">
         <v>150</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="18">
         <v>30</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="19">
         <f>E49</f>
         <v>45910</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="20">
         <f t="shared" si="13"/>
         <v>45940</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="26.25" x14ac:dyDescent="0.35">
-      <c r="A107" s="9" t="s">
+      <c r="A107" s="5" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>